<commit_message>
fix bugs, add dashboard, users, seller analytics
</commit_message>
<xml_diff>
--- a/server/docs/SKLAD.xlsx
+++ b/server/docs/SKLAD.xlsx
@@ -4,14 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="1.01.2023 - 20.12.2023" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="Yillik 2024" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="Oylik 01" state="visible" r:id="rId5"/>
+    <sheet sheetId="3" name="Haftalik 1.01.2024 - 8.01.2024" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="6">
   <si>
     <t>ID</t>
   </si>
@@ -25,28 +27,10 @@
     <t>Sanasi va Vaqti</t>
   </si>
   <si>
-    <t>Svarshikka</t>
-  </si>
-  <si>
-    <t>15 000 so'm</t>
-  </si>
-  <si>
-    <t>19.11.2023 12:43:27</t>
-  </si>
-  <si>
-    <t>Eshmamat Kamaz</t>
-  </si>
-  <si>
-    <t>45 000 so'm</t>
-  </si>
-  <si>
-    <t>19.12.2023 12:43:52</t>
-  </si>
-  <si>
     <t>Umumiy Harajat Summasi</t>
   </si>
   <si>
-    <t>60 000 so'm</t>
+    <t>0 so'm</t>
   </si>
 </sst>
 </file>
@@ -436,13 +420,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -460,39 +444,89 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>